<commit_message>
changes made on 29 aug 2024
</commit_message>
<xml_diff>
--- a/testdata/group_and_user.xlsx
+++ b/testdata/group_and_user.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\eclipse-workspace\Convirza_Automation\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Convirza Automation\Convirza_Automation\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67EE1596-B79F-41C6-BF7F-1D1C7660C490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="group_details" sheetId="1" r:id="rId1"/>
-    <sheet name="user details" sheetId="2" r:id="rId2"/>
+    <sheet name="user_details" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>parent group</t>
   </si>
@@ -37,12 +38,27 @@
   </si>
   <si>
     <t>industryName</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ln</t>
+  </si>
+  <si>
+    <t>usergroup</t>
+  </si>
+  <si>
+    <t>userrole</t>
+  </si>
+  <si>
+    <t>Admin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -353,20 +369,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -374,7 +391,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -388,13 +405,41 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>